<commit_message>
back to excel files
</commit_message>
<xml_diff>
--- a/static/fullbatchresult.xlsx
+++ b/static/fullbatchresult.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/rcmarks2_illinois_edu/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/rcmarks2_illinois_edu/Documents/Desktop/echo-mapping-project/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3E82DC0-A5A6-45D7-B103-60D7357F670B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C3E82DC0-A5A6-45D7-B103-60D7357F670B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E7BDCFA-2950-4D48-A6A1-36A7D7C8149A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AFEF1790-4D40-45A6-9418-EB0467DA389D}"/>
   </bookViews>
@@ -156,20 +156,20 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -181,13 +181,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -524,91 +517,91 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -618,12 +611,12 @@
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:N1"/>
   </mergeCells>
-  <conditionalFormatting sqref="J3:J1048576">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",J3)))</formula>
+  <conditionalFormatting sqref="J4:J1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",J3)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>